<commit_message>
Moved Screendata to Notes folder. Added notes to pointer documentation. Started documentation of Bomberman 5 Gold comparison.
</commit_message>
<xml_diff>
--- a/Notes/SBM5_PointerTableDocumentation.xlsx
+++ b/Notes/SBM5_PointerTableDocumentation.xlsx
@@ -2,24 +2,59 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GoogleDrive\SBM5\Notes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\OneDrive\Home\ROM Hacking\SBM5_SFC_EN\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="29952" windowHeight="10368"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="29955" windowHeight="10365" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="SBM5_PointerTableDocumentation" sheetId="1" r:id="rId1"/>
+    <sheet name="Graphics Pointer Table" sheetId="1" r:id="rId1"/>
+    <sheet name="Menu Text Pointer Table" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Daniel Burgess</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>DackR:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+This is the location of the Pointer. PC Offset.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1887" uniqueCount="1131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1895" uniqueCount="1132">
   <si>
     <t>Pointer Offset</t>
   </si>
@@ -3412,13 +3447,16 @@
   </si>
   <si>
     <t>Battle Mode Menu Title - Single? Tag? Move to DF4B82 (1F4B82 PC)</t>
+  </si>
+  <si>
+    <t>11A000</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3552,6 +3590,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="33">
@@ -4229,26 +4280,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G292"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="B90" sqref="B90"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="12.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="71.77734375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="6.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="71.7109375" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4271,7 +4322,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -4291,7 +4342,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -4311,7 +4362,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
@@ -4331,7 +4382,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
@@ -4351,7 +4402,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
@@ -4371,7 +4422,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>26</v>
       </c>
@@ -4391,7 +4442,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>29</v>
       </c>
@@ -4411,7 +4462,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>32</v>
       </c>
@@ -4431,7 +4482,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>36</v>
       </c>
@@ -4451,7 +4502,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>39</v>
       </c>
@@ -4471,7 +4522,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>42</v>
       </c>
@@ -4491,7 +4542,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>46</v>
       </c>
@@ -4511,7 +4562,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>49</v>
       </c>
@@ -4531,7 +4582,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>52</v>
       </c>
@@ -4551,7 +4602,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>56</v>
       </c>
@@ -4571,7 +4622,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>59</v>
       </c>
@@ -4591,7 +4642,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>62</v>
       </c>
@@ -4611,7 +4662,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>65</v>
       </c>
@@ -4631,7 +4682,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>69</v>
       </c>
@@ -4651,7 +4702,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>72</v>
       </c>
@@ -4671,7 +4722,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>76</v>
       </c>
@@ -4691,7 +4742,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>79</v>
       </c>
@@ -4711,7 +4762,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>83</v>
       </c>
@@ -4731,7 +4782,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>86</v>
       </c>
@@ -4751,7 +4802,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>90</v>
       </c>
@@ -4771,7 +4822,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>93</v>
       </c>
@@ -4791,7 +4842,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>97</v>
       </c>
@@ -4811,7 +4862,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>100</v>
       </c>
@@ -4831,7 +4882,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>104</v>
       </c>
@@ -4851,7 +4902,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>107</v>
       </c>
@@ -4871,7 +4922,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>110</v>
       </c>
@@ -4891,7 +4942,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>114</v>
       </c>
@@ -4911,7 +4962,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>118</v>
       </c>
@@ -4931,7 +4982,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>121</v>
       </c>
@@ -4951,7 +5002,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>125</v>
       </c>
@@ -4971,7 +5022,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>128</v>
       </c>
@@ -4991,7 +5042,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>134</v>
       </c>
@@ -5014,7 +5065,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>138</v>
       </c>
@@ -5034,7 +5085,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>141</v>
       </c>
@@ -5054,7 +5105,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>145</v>
       </c>
@@ -5074,7 +5125,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>148</v>
       </c>
@@ -5094,7 +5145,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>151</v>
       </c>
@@ -5114,7 +5165,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>155</v>
       </c>
@@ -5134,7 +5185,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>158</v>
       </c>
@@ -5154,7 +5205,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>162</v>
       </c>
@@ -5174,7 +5225,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>166</v>
       </c>
@@ -5194,7 +5245,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>170</v>
       </c>
@@ -5214,7 +5265,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>173</v>
       </c>
@@ -5234,7 +5285,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>177</v>
       </c>
@@ -5254,7 +5305,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>181</v>
       </c>
@@ -5274,7 +5325,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>185</v>
       </c>
@@ -5294,7 +5345,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>189</v>
       </c>
@@ -5314,7 +5365,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>192</v>
       </c>
@@ -5334,7 +5385,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>195</v>
       </c>
@@ -5354,7 +5405,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>199</v>
       </c>
@@ -5374,7 +5425,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>203</v>
       </c>
@@ -5394,7 +5445,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>207</v>
       </c>
@@ -5414,7 +5465,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>210</v>
       </c>
@@ -5434,7 +5485,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>214</v>
       </c>
@@ -5454,7 +5505,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>217</v>
       </c>
@@ -5474,7 +5525,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>221</v>
       </c>
@@ -5494,7 +5545,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>225</v>
       </c>
@@ -5514,7 +5565,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>229</v>
       </c>
@@ -5534,7 +5585,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>233</v>
       </c>
@@ -5554,7 +5605,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>237</v>
       </c>
@@ -5574,7 +5625,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>241</v>
       </c>
@@ -5594,7 +5645,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>245</v>
       </c>
@@ -5614,7 +5665,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>249</v>
       </c>
@@ -5634,7 +5685,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>253</v>
       </c>
@@ -5654,7 +5705,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>257</v>
       </c>
@@ -5674,7 +5725,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>260</v>
       </c>
@@ -5694,7 +5745,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>263</v>
       </c>
@@ -5714,7 +5765,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>266</v>
       </c>
@@ -5734,7 +5785,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>269</v>
       </c>
@@ -5754,7 +5805,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>272</v>
       </c>
@@ -5774,7 +5825,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>275</v>
       </c>
@@ -5794,7 +5845,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>278</v>
       </c>
@@ -5814,7 +5865,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>281</v>
       </c>
@@ -5834,7 +5885,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>284</v>
       </c>
@@ -5854,7 +5905,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>288</v>
       </c>
@@ -5874,7 +5925,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>291</v>
       </c>
@@ -5894,7 +5945,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>295</v>
       </c>
@@ -5914,7 +5965,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>298</v>
       </c>
@@ -5934,7 +5985,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>301</v>
       </c>
@@ -5954,7 +6005,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>305</v>
       </c>
@@ -5974,7 +6025,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>308</v>
       </c>
@@ -5994,7 +6045,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>311</v>
       </c>
@@ -6017,7 +6068,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>314</v>
       </c>
@@ -6040,7 +6091,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>318</v>
       </c>
@@ -6063,7 +6114,7 @@
         <v>1055</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>321</v>
       </c>
@@ -6086,7 +6137,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>324</v>
       </c>
@@ -6109,7 +6160,7 @@
         <v>1053</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>328</v>
       </c>
@@ -6132,7 +6183,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>332</v>
       </c>
@@ -6155,7 +6206,7 @@
         <v>1015</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>335</v>
       </c>
@@ -6178,7 +6229,7 @@
         <v>1012</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>340</v>
       </c>
@@ -6201,7 +6252,7 @@
         <v>1051</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>343</v>
       </c>
@@ -6224,7 +6275,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>348</v>
       </c>
@@ -6247,7 +6298,7 @@
         <v>1049</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>353</v>
       </c>
@@ -6270,7 +6321,7 @@
         <v>1048</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>357</v>
       </c>
@@ -6293,7 +6344,7 @@
         <v>1047</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>361</v>
       </c>
@@ -6316,7 +6367,7 @@
         <v>1046</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>365</v>
       </c>
@@ -6339,7 +6390,7 @@
         <v>1045</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>368</v>
       </c>
@@ -6362,7 +6413,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>372</v>
       </c>
@@ -6385,7 +6436,7 @@
         <v>1042</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>375</v>
       </c>
@@ -6408,7 +6459,7 @@
         <v>1043</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>378</v>
       </c>
@@ -6431,7 +6482,7 @@
         <v>1041</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>382</v>
       </c>
@@ -6454,7 +6505,7 @@
         <v>1014</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>385</v>
       </c>
@@ -6477,7 +6528,7 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>389</v>
       </c>
@@ -6500,7 +6551,7 @@
         <v>1013</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>393</v>
       </c>
@@ -6523,7 +6574,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>397</v>
       </c>
@@ -6546,7 +6597,7 @@
         <v>1038</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>401</v>
       </c>
@@ -6569,7 +6620,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>404</v>
       </c>
@@ -6592,7 +6643,7 @@
         <v>1036</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>408</v>
       </c>
@@ -6615,7 +6666,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>411</v>
       </c>
@@ -6638,7 +6689,7 @@
         <v>1034</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>414</v>
       </c>
@@ -6661,7 +6712,7 @@
         <v>1033</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>418</v>
       </c>
@@ -6684,7 +6735,7 @@
         <v>1032</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>421</v>
       </c>
@@ -6707,7 +6758,7 @@
         <v>1031</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>424</v>
       </c>
@@ -6730,7 +6781,7 @@
         <v>1030</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>427</v>
       </c>
@@ -6753,7 +6804,7 @@
         <v>1019</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>430</v>
       </c>
@@ -6776,7 +6827,7 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>433</v>
       </c>
@@ -6799,7 +6850,7 @@
         <v>1123</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>436</v>
       </c>
@@ -6822,7 +6873,7 @@
         <v>1122</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>439</v>
       </c>
@@ -6845,7 +6896,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>443</v>
       </c>
@@ -6868,7 +6919,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>446</v>
       </c>
@@ -6891,7 +6942,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>449</v>
       </c>
@@ -6914,7 +6965,7 @@
         <v>1119</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>453</v>
       </c>
@@ -6937,7 +6988,7 @@
         <v>1021</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>457</v>
       </c>
@@ -6960,7 +7011,7 @@
         <v>1022</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>461</v>
       </c>
@@ -6983,7 +7034,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>465</v>
       </c>
@@ -7006,7 +7057,7 @@
         <v>1121</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>468</v>
       </c>
@@ -7029,7 +7080,7 @@
         <v>1120</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>472</v>
       </c>
@@ -7052,7 +7103,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>476</v>
       </c>
@@ -7075,7 +7126,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>480</v>
       </c>
@@ -7098,7 +7149,7 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>484</v>
       </c>
@@ -7121,7 +7172,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>487</v>
       </c>
@@ -7144,7 +7195,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>490</v>
       </c>
@@ -7167,7 +7218,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>494</v>
       </c>
@@ -7190,7 +7241,7 @@
         <v>1029</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>498</v>
       </c>
@@ -7210,7 +7261,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>501</v>
       </c>
@@ -7230,7 +7281,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>504</v>
       </c>
@@ -7250,7 +7301,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>507</v>
       </c>
@@ -7270,7 +7321,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>510</v>
       </c>
@@ -7290,7 +7341,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>514</v>
       </c>
@@ -7310,7 +7361,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>518</v>
       </c>
@@ -7330,7 +7381,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
         <v>521</v>
       </c>
@@ -7350,7 +7401,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>524</v>
       </c>
@@ -7373,7 +7424,7 @@
         <v>1080</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
         <v>528</v>
       </c>
@@ -7396,7 +7447,7 @@
         <v>1079</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>531</v>
       </c>
@@ -7419,7 +7470,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
         <v>535</v>
       </c>
@@ -7442,7 +7493,7 @@
         <v>1077</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>538</v>
       </c>
@@ -7465,7 +7516,7 @@
         <v>1076</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>541</v>
       </c>
@@ -7488,7 +7539,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>544</v>
       </c>
@@ -7511,7 +7562,7 @@
         <v>1074</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>548</v>
       </c>
@@ -7534,7 +7585,7 @@
         <v>1073</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>552</v>
       </c>
@@ -7557,7 +7608,7 @@
         <v>1072</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>555</v>
       </c>
@@ -7580,7 +7631,7 @@
         <v>1071</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>559</v>
       </c>
@@ -7603,7 +7654,7 @@
         <v>1017</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>562</v>
       </c>
@@ -7626,7 +7677,7 @@
         <v>1070</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>565</v>
       </c>
@@ -7649,7 +7700,7 @@
         <v>1069</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>568</v>
       </c>
@@ -7672,7 +7723,7 @@
         <v>1068</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>572</v>
       </c>
@@ -7695,7 +7746,7 @@
         <v>1067</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>575</v>
       </c>
@@ -7718,7 +7769,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>578</v>
       </c>
@@ -7741,7 +7792,7 @@
         <v>1065</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>582</v>
       </c>
@@ -7764,7 +7815,7 @@
         <v>1064</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>585</v>
       </c>
@@ -7787,7 +7838,7 @@
         <v>1063</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>589</v>
       </c>
@@ -7810,7 +7861,7 @@
         <v>1062</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>593</v>
       </c>
@@ -7833,7 +7884,7 @@
         <v>1018</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
         <v>597</v>
       </c>
@@ -7856,7 +7907,7 @@
         <v>1061</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>600</v>
       </c>
@@ -7879,7 +7930,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
         <v>603</v>
       </c>
@@ -7902,7 +7953,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
         <v>606</v>
       </c>
@@ -7925,7 +7976,7 @@
         <v>1058</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
         <v>610</v>
       </c>
@@ -7948,7 +7999,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>614</v>
       </c>
@@ -7971,7 +8022,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
         <v>617</v>
       </c>
@@ -7994,7 +8045,7 @@
         <v>1082</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
         <v>621</v>
       </c>
@@ -8017,7 +8068,7 @@
         <v>1083</v>
       </c>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
         <v>625</v>
       </c>
@@ -8040,7 +8091,7 @@
         <v>1084</v>
       </c>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
         <v>628</v>
       </c>
@@ -8063,7 +8114,7 @@
         <v>1085</v>
       </c>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
         <v>631</v>
       </c>
@@ -8086,7 +8137,7 @@
         <v>1086</v>
       </c>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
         <v>634</v>
       </c>
@@ -8109,7 +8160,7 @@
         <v>1087</v>
       </c>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
         <v>638</v>
       </c>
@@ -8132,7 +8183,7 @@
         <v>1088</v>
       </c>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
         <v>641</v>
       </c>
@@ -8155,7 +8206,7 @@
         <v>1089</v>
       </c>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
         <v>645</v>
       </c>
@@ -8178,7 +8229,7 @@
         <v>1090</v>
       </c>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
         <v>648</v>
       </c>
@@ -8201,7 +8252,7 @@
         <v>1091</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
         <v>651</v>
       </c>
@@ -8224,7 +8275,7 @@
         <v>1092</v>
       </c>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
         <v>655</v>
       </c>
@@ -8247,7 +8298,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
         <v>658</v>
       </c>
@@ -8270,7 +8321,7 @@
         <v>1094</v>
       </c>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
         <v>662</v>
       </c>
@@ -8293,7 +8344,7 @@
         <v>1095</v>
       </c>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
         <v>665</v>
       </c>
@@ -8316,7 +8367,7 @@
         <v>1096</v>
       </c>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
         <v>668</v>
       </c>
@@ -8339,7 +8390,7 @@
         <v>1097</v>
       </c>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
         <v>671</v>
       </c>
@@ -8362,7 +8413,7 @@
         <v>1098</v>
       </c>
     </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
         <v>675</v>
       </c>
@@ -8385,7 +8436,7 @@
         <v>1099</v>
       </c>
     </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
         <v>678</v>
       </c>
@@ -8408,7 +8459,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
         <v>681</v>
       </c>
@@ -8431,7 +8482,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
         <v>684</v>
       </c>
@@ -8454,7 +8505,7 @@
         <v>1102</v>
       </c>
     </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
         <v>687</v>
       </c>
@@ -8477,7 +8528,7 @@
         <v>1103</v>
       </c>
     </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
         <v>691</v>
       </c>
@@ -8500,7 +8551,7 @@
         <v>1104</v>
       </c>
     </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
         <v>694</v>
       </c>
@@ -8523,7 +8574,7 @@
         <v>1105</v>
       </c>
     </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
         <v>697</v>
       </c>
@@ -8546,7 +8597,7 @@
         <v>1106</v>
       </c>
     </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
         <v>701</v>
       </c>
@@ -8569,7 +8620,7 @@
         <v>1107</v>
       </c>
     </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
         <v>704</v>
       </c>
@@ -8592,7 +8643,7 @@
         <v>1108</v>
       </c>
     </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
         <v>707</v>
       </c>
@@ -8615,7 +8666,7 @@
         <v>1109</v>
       </c>
     </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
         <v>710</v>
       </c>
@@ -8638,7 +8689,7 @@
         <v>1012</v>
       </c>
     </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
         <v>713</v>
       </c>
@@ -8661,7 +8712,7 @@
         <v>1110</v>
       </c>
     </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
         <v>716</v>
       </c>
@@ -8684,7 +8735,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
         <v>719</v>
       </c>
@@ -8707,7 +8758,7 @@
         <v>1128</v>
       </c>
     </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
         <v>723</v>
       </c>
@@ -8730,7 +8781,7 @@
         <v>1130</v>
       </c>
     </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
         <v>727</v>
       </c>
@@ -8753,7 +8804,7 @@
         <v>1111</v>
       </c>
     </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
         <v>731</v>
       </c>
@@ -8776,7 +8827,7 @@
         <v>1111</v>
       </c>
     </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
         <v>734</v>
       </c>
@@ -8799,7 +8850,7 @@
         <v>1111</v>
       </c>
     </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A211" s="1" t="s">
         <v>738</v>
       </c>
@@ -8822,7 +8873,7 @@
         <v>1111</v>
       </c>
     </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
         <v>741</v>
       </c>
@@ -8845,7 +8896,7 @@
         <v>1111</v>
       </c>
     </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
         <v>744</v>
       </c>
@@ -8868,7 +8919,7 @@
         <v>1111</v>
       </c>
     </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
         <v>748</v>
       </c>
@@ -8891,7 +8942,7 @@
         <v>1111</v>
       </c>
     </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
         <v>751</v>
       </c>
@@ -8914,7 +8965,7 @@
         <v>1112</v>
       </c>
     </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
         <v>754</v>
       </c>
@@ -8937,7 +8988,7 @@
         <v>1111</v>
       </c>
     </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
         <v>757</v>
       </c>
@@ -8960,7 +9011,7 @@
         <v>1111</v>
       </c>
     </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
         <v>761</v>
       </c>
@@ -8983,7 +9034,7 @@
         <v>1111</v>
       </c>
     </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A219" s="1" t="s">
         <v>764</v>
       </c>
@@ -9006,7 +9057,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
         <v>767</v>
       </c>
@@ -9029,7 +9080,7 @@
         <v>1111</v>
       </c>
     </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
         <v>770</v>
       </c>
@@ -9052,7 +9103,7 @@
         <v>1113</v>
       </c>
     </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A222" s="1" t="s">
         <v>774</v>
       </c>
@@ -9075,7 +9126,7 @@
         <v>1113</v>
       </c>
     </row>
-    <row r="223" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
         <v>777</v>
       </c>
@@ -9098,7 +9149,7 @@
         <v>1114</v>
       </c>
     </row>
-    <row r="224" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
         <v>780</v>
       </c>
@@ -9121,7 +9172,7 @@
         <v>1080</v>
       </c>
     </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A225" s="1" t="s">
         <v>784</v>
       </c>
@@ -9144,7 +9195,7 @@
         <v>1080</v>
       </c>
     </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
         <v>788</v>
       </c>
@@ -9164,7 +9215,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
         <v>791</v>
       </c>
@@ -9184,7 +9235,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="228" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
         <v>794</v>
       </c>
@@ -9204,7 +9255,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A229" s="1" t="s">
         <v>798</v>
       </c>
@@ -9224,7 +9275,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
         <v>801</v>
       </c>
@@ -9244,7 +9295,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A231" s="1" t="s">
         <v>805</v>
       </c>
@@ -9264,7 +9315,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A232" s="1" t="s">
         <v>809</v>
       </c>
@@ -9284,7 +9335,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="233" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A233" s="1" t="s">
         <v>812</v>
       </c>
@@ -9304,7 +9355,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="234" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A234" s="1" t="s">
         <v>815</v>
       </c>
@@ -9324,7 +9375,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="235" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A235" s="1" t="s">
         <v>819</v>
       </c>
@@ -9344,7 +9395,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="236" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
         <v>823</v>
       </c>
@@ -9364,7 +9415,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="237" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A237" s="1" t="s">
         <v>826</v>
       </c>
@@ -9384,7 +9435,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="238" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
         <v>830</v>
       </c>
@@ -9404,7 +9455,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="239" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A239" s="1" t="s">
         <v>834</v>
       </c>
@@ -9424,7 +9475,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="240" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A240" s="1" t="s">
         <v>838</v>
       </c>
@@ -9444,7 +9495,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="241" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A241" s="1" t="s">
         <v>842</v>
       </c>
@@ -9464,7 +9515,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="242" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A242" s="1" t="s">
         <v>845</v>
       </c>
@@ -9484,7 +9535,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="243" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A243" s="1" t="s">
         <v>848</v>
       </c>
@@ -9504,7 +9555,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="244" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A244" s="1" t="s">
         <v>852</v>
       </c>
@@ -9524,7 +9575,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="245" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A245" s="1" t="s">
         <v>855</v>
       </c>
@@ -9544,7 +9595,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="246" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A246" s="1" t="s">
         <v>859</v>
       </c>
@@ -9564,7 +9615,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="247" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A247" s="1" t="s">
         <v>863</v>
       </c>
@@ -9587,7 +9638,7 @@
         <v>1115</v>
       </c>
     </row>
-    <row r="248" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A248" s="1" t="s">
         <v>867</v>
       </c>
@@ -9607,7 +9658,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="249" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A249" s="1" t="s">
         <v>870</v>
       </c>
@@ -9630,7 +9681,7 @@
         <v>1116</v>
       </c>
     </row>
-    <row r="250" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A250" s="1" t="s">
         <v>874</v>
       </c>
@@ -9653,7 +9704,7 @@
         <v>1117</v>
       </c>
     </row>
-    <row r="251" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A251" s="1" t="s">
         <v>878</v>
       </c>
@@ -9673,7 +9724,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="252" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A252" s="1" t="s">
         <v>882</v>
       </c>
@@ -9693,7 +9744,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="253" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A253" s="1" t="s">
         <v>886</v>
       </c>
@@ -9713,7 +9764,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="254" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A254" s="1" t="s">
         <v>889</v>
       </c>
@@ -9733,7 +9784,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="255" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A255" s="1" t="s">
         <v>893</v>
       </c>
@@ -9753,7 +9804,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="256" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A256" s="1" t="s">
         <v>896</v>
       </c>
@@ -9773,7 +9824,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="257" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A257" s="1" t="s">
         <v>900</v>
       </c>
@@ -9793,7 +9844,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="258" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A258" s="1" t="s">
         <v>903</v>
       </c>
@@ -9813,7 +9864,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="259" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A259" s="1" t="s">
         <v>907</v>
       </c>
@@ -9833,7 +9884,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="260" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A260" s="1" t="s">
         <v>910</v>
       </c>
@@ -9853,7 +9904,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="261" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A261" s="1" t="s">
         <v>913</v>
       </c>
@@ -9873,7 +9924,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="262" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A262" s="1" t="s">
         <v>916</v>
       </c>
@@ -9893,7 +9944,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="263" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A263" s="1" t="s">
         <v>919</v>
       </c>
@@ -9913,7 +9964,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="264" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A264" s="1" t="s">
         <v>922</v>
       </c>
@@ -9933,7 +9984,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="265" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A265" s="1" t="s">
         <v>925</v>
       </c>
@@ -9953,7 +10004,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="266" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A266" s="1" t="s">
         <v>928</v>
       </c>
@@ -9973,7 +10024,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="267" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A267" s="1" t="s">
         <v>931</v>
       </c>
@@ -9993,7 +10044,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="268" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
         <v>934</v>
       </c>
@@ -10013,7 +10064,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="269" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A269" s="1" t="s">
         <v>937</v>
       </c>
@@ -10033,7 +10084,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="270" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A270" s="1" t="s">
         <v>940</v>
       </c>
@@ -10053,7 +10104,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="271" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A271" s="1" t="s">
         <v>943</v>
       </c>
@@ -10073,7 +10124,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="272" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A272" s="1" t="s">
         <v>946</v>
       </c>
@@ -10093,7 +10144,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="273" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A273" s="1" t="s">
         <v>949</v>
       </c>
@@ -10113,7 +10164,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="274" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A274" s="1" t="s">
         <v>952</v>
       </c>
@@ -10133,7 +10184,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="275" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A275" s="1" t="s">
         <v>955</v>
       </c>
@@ -10153,7 +10204,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="276" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A276" s="1" t="s">
         <v>958</v>
       </c>
@@ -10173,7 +10224,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="277" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A277" s="1" t="s">
         <v>961</v>
       </c>
@@ -10193,7 +10244,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="278" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A278" s="1" t="s">
         <v>964</v>
       </c>
@@ -10213,7 +10264,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="279" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A279" s="1" t="s">
         <v>967</v>
       </c>
@@ -10233,7 +10284,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="280" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A280" s="1" t="s">
         <v>970</v>
       </c>
@@ -10253,7 +10304,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="281" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A281" s="1" t="s">
         <v>973</v>
       </c>
@@ -10273,7 +10324,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="282" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A282" s="1" t="s">
         <v>976</v>
       </c>
@@ -10293,7 +10344,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="283" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A283" s="1" t="s">
         <v>979</v>
       </c>
@@ -10313,7 +10364,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="284" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A284" s="1" t="s">
         <v>982</v>
       </c>
@@ -10333,7 +10384,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="285" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A285" s="1" t="s">
         <v>986</v>
       </c>
@@ -10353,7 +10404,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="286" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A286" s="1" t="s">
         <v>989</v>
       </c>
@@ -10373,7 +10424,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="287" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A287" s="1" t="s">
         <v>992</v>
       </c>
@@ -10393,7 +10444,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="288" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A288" s="1" t="s">
         <v>995</v>
       </c>
@@ -10413,7 +10464,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="289" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A289" s="1" t="s">
         <v>998</v>
       </c>
@@ -10433,7 +10484,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="290" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A290" s="1" t="s">
         <v>1001</v>
       </c>
@@ -10453,7 +10504,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="291" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A291" s="1" t="s">
         <v>1004</v>
       </c>
@@ -10473,7 +10524,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="292" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A292" s="1" t="s">
         <v>1007</v>
       </c>
@@ -10499,5 +10550,58 @@
   <ignoredErrors>
     <ignoredError sqref="C2:E2" numberStoredAsText="1"/>
   </ignoredErrors>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="84.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1010</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1131</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Automatically generated Text Pointer table documentation.
</commit_message>
<xml_diff>
--- a/Notes/SBM5_PointerTableDocumentation.xlsx
+++ b/Notes/SBM5_PointerTableDocumentation.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="29955" windowHeight="10365" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="29955" windowHeight="10365"/>
   </bookViews>
   <sheets>
     <sheet name="Graphics Pointer Table" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1895" uniqueCount="1132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1896" uniqueCount="1133">
   <si>
     <t>Pointer Offset</t>
   </si>
@@ -3450,6 +3450,9 @@
   </si>
   <si>
     <t>11A000</t>
+  </si>
+  <si>
+    <t>Type 85 is uncompressed, so these sections need to be re-extracted.</t>
   </si>
 </sst>
 </file>
@@ -4283,10 +4286,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G292"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4341,6 +4344,9 @@
       <c r="F2" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="G2" s="4" t="s">
+        <v>1132</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -10558,7 +10564,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Reorganized some things. Trying to figure out the tilemap compression.
</commit_message>
<xml_diff>
--- a/Notes/SBM5_PointerTableDocumentation.xlsx
+++ b/Notes/SBM5_PointerTableDocumentation.xlsx
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3140" uniqueCount="2379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3142" uniqueCount="2381">
   <si>
     <t>Pointer Offset</t>
   </si>
@@ -7213,6 +7213,12 @@
   </si>
   <si>
     <t>Original Pointer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Match Rules - Screen Data and Menu Heading </t>
+  </si>
+  <si>
+    <t>Character Select - Screen Data and Menu Heading</t>
   </si>
 </sst>
 </file>
@@ -8052,9 +8058,9 @@
   <dimension ref="A1:G292"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A164" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
+      <selection pane="bottomLeft" activeCell="G167" sqref="G167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14329,8 +14335,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H249"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="B120" sqref="B120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16848,6 +16854,9 @@
         <v>2242</v>
       </c>
       <c r="G119" s="5"/>
+      <c r="H119" s="5" t="s">
+        <v>2379</v>
+      </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120">
@@ -17049,7 +17058,7 @@
       </c>
       <c r="G128" s="5"/>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>127</v>
       </c>
@@ -17070,7 +17079,7 @@
       </c>
       <c r="G129" s="5"/>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>128</v>
       </c>
@@ -17091,7 +17100,7 @@
       </c>
       <c r="G130" s="5"/>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>129</v>
       </c>
@@ -17112,7 +17121,7 @@
       </c>
       <c r="G131" s="5"/>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>130</v>
       </c>
@@ -17133,7 +17142,7 @@
       </c>
       <c r="G132" s="5"/>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>131</v>
       </c>
@@ -17154,7 +17163,7 @@
       </c>
       <c r="G133" s="5"/>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>132</v>
       </c>
@@ -17175,7 +17184,7 @@
       </c>
       <c r="G134" s="5"/>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>133</v>
       </c>
@@ -17196,7 +17205,7 @@
       </c>
       <c r="G135" s="5"/>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>134</v>
       </c>
@@ -17217,7 +17226,7 @@
       </c>
       <c r="G136" s="5"/>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>135</v>
       </c>
@@ -17237,8 +17246,11 @@
         <v>2260</v>
       </c>
       <c r="G137" s="5"/>
-    </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H137" s="5" t="s">
+        <v>2380</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>136</v>
       </c>
@@ -17259,7 +17271,7 @@
       </c>
       <c r="G138" s="5"/>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>137</v>
       </c>
@@ -17280,7 +17292,7 @@
       </c>
       <c r="G139" s="5"/>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>138</v>
       </c>
@@ -17301,7 +17313,7 @@
       </c>
       <c r="G140" s="5"/>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>139</v>
       </c>
@@ -17322,7 +17334,7 @@
       </c>
       <c r="G141" s="5"/>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>140</v>
       </c>
@@ -17343,7 +17355,7 @@
       </c>
       <c r="G142" s="5"/>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>141</v>
       </c>
@@ -17364,7 +17376,7 @@
       </c>
       <c r="G143" s="5"/>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>142</v>
       </c>

</xml_diff>